<commit_message>
Added tests, finished generate sites, and confirmed import spreadsheet field values
</commit_message>
<xml_diff>
--- a/bulk_import_tool/IMM import template - test.xlsx
+++ b/bulk_import_tool/IMM import template - test.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="IMM_template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -349,9 +349,6 @@
     <t>GeographicSite.ecoprovince</t>
   </si>
   <si>
-    <t>GeographicSite.fossile_ref_no</t>
-  </si>
-  <si>
     <t>GeographicSite.mine_name</t>
   </si>
   <si>
@@ -757,9 +754,6 @@
     <t>BotanyItem.partial_specimen</t>
   </si>
   <si>
-    <t>Phenology.phenology_cd</t>
-  </si>
-  <si>
     <t>[DISCIPLINE].quantity</t>
   </si>
   <si>
@@ -808,18 +802,12 @@
     <t>MammalogyItem.breeding</t>
   </si>
   <si>
-    <t>MammalogyItem.odd_colour_form</t>
-  </si>
-  <si>
     <t>SexType.sex_cd</t>
   </si>
   <si>
     <t>MeasurementType.measurement_cd</t>
   </si>
   <si>
-    <t>UnitType.unit.cd</t>
-  </si>
-  <si>
     <t>Measurement.m_value</t>
   </si>
   <si>
@@ -935,6 +923,18 @@
   </si>
   <si>
     <t>Specimen Notes test</t>
+  </si>
+  <si>
+    <t>GeographicSite.fossile_ref_num</t>
+  </si>
+  <si>
+    <t>PhenologyType.phenology_cd</t>
+  </si>
+  <si>
+    <t>MammalogyItem.ood_colour_form</t>
+  </si>
+  <si>
+    <t>UnitType.unit_cd</t>
   </si>
 </sst>
 </file>
@@ -1379,9 +1379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DF1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="DV1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="DN4" sqref="DN4"/>
+      <selection pane="bottomLeft" activeCell="ED3" sqref="ED3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,7 +1472,7 @@
       <c r="AC1" s="20"/>
       <c r="AD1" s="20"/>
       <c r="AE1" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF1" s="21"/>
       <c r="AG1" s="21"/>
@@ -1517,13 +1517,13 @@
       <c r="BT1" s="21"/>
       <c r="BU1" s="21"/>
       <c r="BV1" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BW1" s="22"/>
       <c r="BX1" s="22"/>
       <c r="BY1" s="22"/>
       <c r="BZ1" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="CA1" s="23"/>
       <c r="CB1" s="23"/>
@@ -1559,7 +1559,7 @@
       <c r="DF1" s="23"/>
       <c r="DG1" s="23"/>
       <c r="DH1" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="DI1" s="24"/>
       <c r="DJ1" s="24"/>
@@ -1578,7 +1578,7 @@
       <c r="DW1" s="24"/>
       <c r="DX1" s="24"/>
       <c r="DY1" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="DZ1" s="18"/>
       <c r="EA1" s="18"/>
@@ -1800,202 +1800,202 @@
         <v>99</v>
       </c>
       <c r="BS2" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="BT2" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="BU2" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="BV2" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BW2" s="4" t="s">
         <v>83</v>
       </c>
       <c r="BX2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BY2" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="BY2" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="BZ2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="CA2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="CA2" s="2" t="s">
+      <c r="CB2" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="CB2" s="2" t="s">
+      <c r="CC2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="CC2" s="2" t="s">
+      <c r="CD2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="CD2" s="2" t="s">
+      <c r="CE2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="CE2" s="2" t="s">
+      <c r="CF2" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="CF2" s="2" t="s">
+      <c r="CG2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="CG2" s="2" t="s">
+      <c r="CH2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="CH2" s="2" t="s">
+      <c r="CI2" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="CI2" s="2" t="s">
+      <c r="CJ2" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="CJ2" s="2" t="s">
+      <c r="CK2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="CK2" s="2" t="s">
+      <c r="CL2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="CL2" s="2" t="s">
+      <c r="CM2" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="CM2" s="2" t="s">
+      <c r="CN2" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="CN2" s="2" t="s">
+      <c r="CO2" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="CO2" s="2" t="s">
+      <c r="CP2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="CP2" s="2" t="s">
+      <c r="CQ2" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="CQ2" s="2" t="s">
+      <c r="CR2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="CR2" s="2" t="s">
+      <c r="CS2" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="CS2" s="2" t="s">
+      <c r="CT2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="CT2" s="2" t="s">
+      <c r="CU2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="CU2" s="2" t="s">
+      <c r="CV2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="CV2" s="2" t="s">
+      <c r="CW2" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="CW2" s="2" t="s">
+      <c r="CX2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="CX2" s="2" t="s">
+      <c r="CY2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="CY2" s="2" t="s">
+      <c r="CZ2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="CZ2" s="2" t="s">
+      <c r="DA2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="DA2" s="2" t="s">
+      <c r="DB2" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="DB2" s="2" t="s">
+      <c r="DC2" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DD2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="DE2" s="2" t="s">
+      <c r="DF2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="DF2" s="2" t="s">
+      <c r="DG2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="DG2" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="DH2" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="DI2" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="DI2" s="8" t="s">
+      <c r="DJ2" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="DJ2" s="8" t="s">
+      <c r="DK2" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="DK2" s="8" t="s">
+      <c r="DL2" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="DL2" s="8" t="s">
+      <c r="DM2" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="DM2" s="8" t="s">
+      <c r="DN2" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="DN2" s="8" t="s">
+      <c r="DO2" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="DO2" s="8" t="s">
+      <c r="DP2" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="DP2" s="8" t="s">
+      <c r="DQ2" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="DQ2" s="8" t="s">
+      <c r="DR2" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="DR2" s="8" t="s">
+      <c r="DS2" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="DS2" s="8" t="s">
+      <c r="DT2" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="DT2" s="8" t="s">
+      <c r="DU2" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="DU2" s="8" t="s">
+      <c r="DV2" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="DV2" s="8" t="s">
+      <c r="DW2" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="DW2" s="8" t="s">
+      <c r="DX2" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="DX2" s="8" t="s">
-        <v>236</v>
-      </c>
       <c r="DY2" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="DZ2" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="EA2" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="DZ2" s="7" t="s">
+      <c r="EB2" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="EA2" s="7" t="s">
+      <c r="EC2" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="EB2" s="7" t="s">
+      <c r="ED2" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="EC2" s="7" t="s">
+      <c r="EE2" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="ED2" s="7" t="s">
+      <c r="EF2" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="EE2" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="EF2" s="7" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:136" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2123,327 +2123,327 @@
         <v>110</v>
       </c>
       <c r="AP3" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="AQ3" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AR3" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="AR3" s="11" t="s">
+      <c r="AS3" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AS3" s="11" t="s">
+      <c r="AT3" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="AT3" s="11" t="s">
+      <c r="AU3" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AU3" s="11" t="s">
+      <c r="AV3" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AV3" s="11" t="s">
+      <c r="AW3" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="AX3" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="AX3" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="AY3" s="11" t="s">
         <v>42</v>
       </c>
       <c r="AZ3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="BA3" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="BA3" s="11" t="s">
+      <c r="BB3" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="BB3" s="11" t="s">
+      <c r="BC3" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="BC3" s="11" t="s">
+      <c r="BD3" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="BD3" s="11" t="s">
+      <c r="BE3" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="BE3" s="11" t="s">
+      <c r="BF3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="BF3" s="11" t="s">
+      <c r="BG3" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="BG3" s="11" t="s">
+      <c r="BH3" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="BH3" s="11" t="s">
+      <c r="BI3" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="BI3" s="11" t="s">
+      <c r="BJ3" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="BJ3" s="11" t="s">
+      <c r="BK3" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="BK3" s="11" t="s">
+      <c r="BL3" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="BL3" s="11" t="s">
+      <c r="BM3" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="BM3" s="11" t="s">
+      <c r="BN3" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="BN3" s="11" t="s">
+      <c r="BO3" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="BO3" s="11" t="s">
+      <c r="BP3" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="BP3" s="11" t="s">
+      <c r="BQ3" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="BQ3" s="11" t="s">
+      <c r="BR3" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="BR3" s="11" t="s">
+      <c r="BS3" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="BS3" s="11" t="s">
+      <c r="BT3" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="BT3" s="11" t="s">
+      <c r="BU3" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="BU3" s="11" t="s">
-        <v>141</v>
-      </c>
       <c r="BV3" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="BW3" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="BW3" s="12" t="s">
+      <c r="BX3" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="BX3" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="BY3" s="12" t="s">
         <v>54</v>
       </c>
       <c r="BZ3" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="CA3" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="CA3" s="13" t="s">
+      <c r="CB3" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="CB3" s="13" t="s">
+      <c r="CC3" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="CC3" s="13" t="s">
+      <c r="CD3" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="CD3" s="13" t="s">
+      <c r="CE3" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="CE3" s="13" t="s">
+      <c r="CF3" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="CF3" s="13" t="s">
+      <c r="CG3" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="CG3" s="13" t="s">
+      <c r="CH3" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="CH3" s="13" t="s">
+      <c r="CI3" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="CI3" s="13" t="s">
+      <c r="CJ3" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="CJ3" s="13" t="s">
+      <c r="CK3" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="CK3" s="13" t="s">
+      <c r="CL3" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="CL3" s="13" t="s">
+      <c r="CM3" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="CM3" s="13" t="s">
+      <c r="CN3" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="CN3" s="13" t="s">
+      <c r="CO3" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="CO3" s="13" t="s">
+      <c r="CP3" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="CP3" s="13" t="s">
+      <c r="CQ3" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="CQ3" s="13" t="s">
+      <c r="CR3" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="CR3" s="13" t="s">
+      <c r="CS3" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="CS3" s="13" t="s">
+      <c r="CT3" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="CT3" s="13" t="s">
+      <c r="CU3" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="CU3" s="13" t="s">
+      <c r="CV3" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="CV3" s="13" t="s">
+      <c r="CW3" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="CW3" s="13" t="s">
+      <c r="CX3" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="CX3" s="13" t="s">
+      <c r="CY3" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="CY3" s="13" t="s">
+      <c r="CZ3" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="CZ3" s="13" t="s">
+      <c r="DA3" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="DA3" s="13" t="s">
+      <c r="DB3" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="DB3" s="13" t="s">
+      <c r="DC3" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="DC3" s="13" t="s">
+      <c r="DD3" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="DD3" s="13" t="s">
+      <c r="DE3" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="DE3" s="13" t="s">
+      <c r="DF3" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="DF3" s="13" t="s">
+      <c r="DG3" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="DG3" s="13" t="s">
-        <v>218</v>
-      </c>
       <c r="DH3" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="DI3" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="DI3" s="14" t="s">
+      <c r="DJ3" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="DJ3" s="14" t="s">
+      <c r="DK3" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="DK3" s="14" t="s">
+      <c r="DL3" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="DL3" s="14" t="s">
+      <c r="DM3" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="DM3" s="14" t="s">
-        <v>242</v>
       </c>
       <c r="DN3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="DO3" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="DP3" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="DP3" s="14" t="s">
+      <c r="DQ3" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="DQ3" s="14" t="s">
+      <c r="DR3" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="DR3" s="14" t="s">
+      <c r="DS3" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="DT3" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="DS3" s="14" t="s">
+      <c r="DU3" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="DT3" s="14" t="s">
+      <c r="DV3" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="DU3" s="14" t="s">
+      <c r="DW3" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="DV3" s="14" t="s">
+      <c r="DX3" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="DW3" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="DX3" s="14" t="s">
-        <v>252</v>
-      </c>
       <c r="DY3" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="DZ3" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="EA3" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="EB3" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="DZ3" s="15" t="s">
+      <c r="EC3" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="EA3" s="15" t="s">
+      <c r="ED3" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="EE3" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="EB3" s="15" t="s">
+      <c r="EF3" s="15" t="s">
         <v>265</v>
-      </c>
-      <c r="EC3" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="ED3" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="EE3" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="EF3" s="15" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I4" s="17">
         <v>43465</v>
       </c>
       <c r="K4" t="s">
+        <v>273</v>
+      </c>
+      <c r="L4" t="s">
+        <v>274</v>
+      </c>
+      <c r="M4" t="s">
+        <v>276</v>
+      </c>
+      <c r="N4" t="s">
         <v>277</v>
       </c>
-      <c r="L4" t="s">
+      <c r="Q4" t="s">
         <v>278</v>
       </c>
-      <c r="M4" t="s">
-        <v>280</v>
-      </c>
-      <c r="N4" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>282</v>
-      </c>
       <c r="W4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="AE4">
         <v>15</v>
@@ -2452,25 +2452,25 @@
         <v>14</v>
       </c>
       <c r="AH4" t="s">
+        <v>280</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>282</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>281</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AW4" t="s">
         <v>284</v>
       </c>
-      <c r="AK4" t="s">
-        <v>286</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT4" t="s">
+      <c r="AX4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>287</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>288</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>292</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>291</v>
       </c>
       <c r="BH4">
         <v>48.419603000000002</v>
@@ -2482,66 +2482,66 @@
         <v>43465</v>
       </c>
       <c r="BX4" t="s">
+        <v>295</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>279</v>
+      </c>
+      <c r="DI4" t="s">
+        <v>300</v>
+      </c>
+      <c r="DJ4" t="s">
         <v>299</v>
       </c>
-      <c r="BY4" t="s">
-        <v>283</v>
-      </c>
-      <c r="DI4" t="s">
-        <v>304</v>
-      </c>
-      <c r="DJ4" t="s">
-        <v>303</v>
-      </c>
       <c r="DM4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="DT4">
         <v>1</v>
       </c>
       <c r="DV4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="DW4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I5" s="17">
         <v>43465</v>
       </c>
       <c r="K5" t="s">
+        <v>273</v>
+      </c>
+      <c r="L5" t="s">
+        <v>275</v>
+      </c>
+      <c r="M5" t="s">
+        <v>276</v>
+      </c>
+      <c r="N5" t="s">
         <v>277</v>
       </c>
-      <c r="L5" t="s">
-        <v>279</v>
-      </c>
-      <c r="M5" t="s">
-        <v>280</v>
-      </c>
-      <c r="N5" t="s">
-        <v>281</v>
-      </c>
       <c r="Q5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="W5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="AE5">
         <v>5</v>
@@ -2550,25 +2550,25 @@
         <v>4</v>
       </c>
       <c r="AH5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="AK5" t="s">
+        <v>282</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>289</v>
+      </c>
+      <c r="AZ5" t="s">
         <v>286</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>289</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>293</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>290</v>
       </c>
       <c r="BH5">
         <v>48.419956999999997</v>
@@ -2580,28 +2580,28 @@
         <v>43465</v>
       </c>
       <c r="BX5" t="s">
+        <v>296</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>297</v>
+      </c>
+      <c r="DI5" t="s">
         <v>300</v>
       </c>
-      <c r="BY5" t="s">
-        <v>301</v>
-      </c>
-      <c r="DI5" t="s">
-        <v>304</v>
-      </c>
       <c r="DJ5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="DM5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="DT5">
         <v>1</v>
       </c>
       <c r="DV5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="DW5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2615,6 +2615,6 @@
     <mergeCell ref="DH1:DX1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Not sure why I need to commit this change
</commit_message>
<xml_diff>
--- a/bulk_import_tool/IMM import template - test.xlsx
+++ b/bulk_import_tool/IMM import template - test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="304">
   <si>
     <t>Catalogue</t>
   </si>
@@ -838,12 +838,6 @@
     <t>INV</t>
   </si>
   <si>
-    <t>Event_01</t>
-  </si>
-  <si>
-    <t>Event_02</t>
-  </si>
-  <si>
     <t>EV1</t>
   </si>
   <si>
@@ -868,12 +862,6 @@
     <t>British Columbia</t>
   </si>
   <si>
-    <t>Site_1</t>
-  </si>
-  <si>
-    <t>Site_2</t>
-  </si>
-  <si>
     <t>Victoria: RBCM Exhibits building</t>
   </si>
   <si>
@@ -935,6 +923,9 @@
   </si>
   <si>
     <t>UnitType.unit_cd</t>
+  </si>
+  <si>
+    <t>EV2</t>
   </si>
 </sst>
 </file>
@@ -1379,9 +1370,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DV1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="ED3" sqref="ED3"/>
+      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,7 +2114,7 @@
         <v>110</v>
       </c>
       <c r="AP3" s="11" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="AQ3" s="11" t="s">
         <v>111</v>
@@ -2366,7 +2357,7 @@
         <v>245</v>
       </c>
       <c r="DS3" s="14" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="DT3" s="14" t="s">
         <v>246</v>
@@ -2390,7 +2381,7 @@
         <v>261</v>
       </c>
       <c r="EA3" s="15" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="EB3" s="15" t="s">
         <v>262</v>
@@ -2399,7 +2390,7 @@
         <v>263</v>
       </c>
       <c r="ED3" s="15" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="EE3" s="15" t="s">
         <v>264</v>
@@ -2410,10 +2401,10 @@
     </row>
     <row r="4" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D4" t="s">
         <v>269</v>
@@ -2430,20 +2421,17 @@
       <c r="K4" t="s">
         <v>273</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>274</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q4" t="s">
         <v>276</v>
       </c>
-      <c r="N4" t="s">
+      <c r="W4" t="s">
         <v>277</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>278</v>
-      </c>
-      <c r="W4" t="s">
-        <v>279</v>
       </c>
       <c r="AE4">
         <v>15</v>
@@ -2452,25 +2440,22 @@
         <v>14</v>
       </c>
       <c r="AH4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AK4" t="s">
         <v>280</v>
       </c>
-      <c r="AK4" t="s">
-        <v>282</v>
-      </c>
       <c r="AL4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AT4" t="s">
         <v>281</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AX4" t="s">
+        <v>284</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>283</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>284</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>288</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>287</v>
       </c>
       <c r="BH4">
         <v>48.419603000000002</v>
@@ -2482,36 +2467,36 @@
         <v>43465</v>
       </c>
       <c r="BX4" t="s">
+        <v>291</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>277</v>
+      </c>
+      <c r="DI4" t="s">
+        <v>296</v>
+      </c>
+      <c r="DJ4" t="s">
         <v>295</v>
       </c>
-      <c r="BY4" t="s">
-        <v>279</v>
-      </c>
-      <c r="DI4" t="s">
-        <v>300</v>
-      </c>
-      <c r="DJ4" t="s">
-        <v>299</v>
-      </c>
       <c r="DM4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="DT4">
         <v>1</v>
       </c>
       <c r="DV4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="DW4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D5" t="s">
         <v>270</v>
@@ -2528,20 +2513,17 @@
       <c r="K5" t="s">
         <v>273</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
+        <v>303</v>
+      </c>
+      <c r="N5" t="s">
         <v>275</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
         <v>276</v>
       </c>
-      <c r="N5" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>278</v>
-      </c>
       <c r="W5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="AE5">
         <v>5</v>
@@ -2550,25 +2532,22 @@
         <v>4</v>
       </c>
       <c r="AH5" t="s">
+        <v>278</v>
+      </c>
+      <c r="AK5" t="s">
         <v>280</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AZ5" t="s">
         <v>282</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>289</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>286</v>
       </c>
       <c r="BH5">
         <v>48.419956999999997</v>
@@ -2580,28 +2559,28 @@
         <v>43465</v>
       </c>
       <c r="BX5" t="s">
+        <v>292</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>293</v>
+      </c>
+      <c r="DI5" t="s">
         <v>296</v>
       </c>
-      <c r="BY5" t="s">
-        <v>297</v>
-      </c>
-      <c r="DI5" t="s">
-        <v>300</v>
-      </c>
       <c r="DJ5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="DM5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="DT5">
         <v>1</v>
       </c>
       <c r="DV5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="DW5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made to _write_spreadsheet, and _generate_event
</commit_message>
<xml_diff>
--- a/bulk_import_tool/IMM import template - test.xlsx
+++ b/bulk_import_tool/IMM import template - test.xlsx
@@ -13,12 +13,12 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Event" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="145621" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="320">
   <si>
     <t>Catalogue</t>
   </si>
@@ -938,34 +938,46 @@
     <t>Person_ids</t>
   </si>
   <si>
+    <t>Evan Harley</t>
+  </si>
+  <si>
+    <t>David Stewart</t>
+  </si>
+  <si>
+    <t>Meg Sugrue</t>
+  </si>
+  <si>
     <t>Heidi Gartner</t>
   </si>
   <si>
     <t>Henry Choong</t>
   </si>
   <si>
-    <t>Evan Harley</t>
-  </si>
-  <si>
     <t>Hugh MacIntosh</t>
   </si>
   <si>
-    <t>Meg Sugrue</t>
-  </si>
-  <si>
-    <t>David Stewart</t>
-  </si>
-  <si>
     <t>Taxon</t>
   </si>
   <si>
     <t>Taxon_ids</t>
   </si>
   <si>
+    <t>Geosite_id</t>
+  </si>
+  <si>
     <t>VS101450</t>
   </si>
   <si>
     <t>VS101451</t>
+  </si>
+  <si>
+    <t>VE17431</t>
+  </si>
+  <si>
+    <t>VE17432</t>
+  </si>
+  <si>
+    <t>Meg Sugrue; David Stewart</t>
   </si>
 </sst>
 </file>
@@ -1063,9 +1075,8 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1084,9 +1095,11 @@
     <xf borderId="1" fillId="7" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="7" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1407,9 +1420,9 @@
   </sheetPr>
   <dimension ref="A1:EF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A4" ySplit="3"/>
-      <selection activeCell="W5" pane="bottomLeft" sqref="W5"/>
+      <selection activeCell="W5" pane="bottomLeft" sqref="A1:EF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1464,846 +1477,846 @@
     <col customWidth="1" max="136" min="136" width="25"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:136">
-      <c r="A1" s="19" t="s">
+    <row customFormat="1" r="1" s="19" spans="1:136">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AE1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="BV1" s="22" t="s">
+      <c r="BV1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="BZ1" s="23" t="s">
+      <c r="BZ1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="DH1" s="24" t="s">
+      <c r="DH1" s="25" t="s">
         <v>5</v>
       </c>
       <c r="DY1" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:136">
-      <c r="A2" s="3" t="s">
+    <row customFormat="1" r="2" s="19" spans="1:136">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="Z2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AA2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AB2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AC2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AD2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AE2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AF2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AG2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AI2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AK2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AL2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AM2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AN2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AO2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AP2" s="5" t="s">
+      <c r="AP2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AR2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AS2" s="5" t="s">
+      <c r="AS2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AT2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AU2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AV2" s="5" t="s">
+      <c r="AV2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AW2" s="5" t="s">
+      <c r="AW2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AX2" s="5" t="s">
+      <c r="AX2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="5" t="s">
+      <c r="AY2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AZ2" s="5" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BA2" s="5" t="s">
+      <c r="BA2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BB2" s="5" t="s">
+      <c r="BB2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BC2" s="5" t="s">
+      <c r="BC2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BD2" s="5" t="s">
+      <c r="BD2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BE2" s="5" t="s">
+      <c r="BE2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BF2" s="5" t="s">
+      <c r="BF2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BG2" s="5" t="s">
+      <c r="BG2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BH2" s="5" t="s">
+      <c r="BH2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BI2" s="5" t="s">
+      <c r="BI2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BJ2" s="5" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BK2" s="5" t="s">
+      <c r="BK2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BL2" s="5" t="s">
+      <c r="BL2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BM2" s="5" t="s">
+      <c r="BM2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BN2" s="5" t="s">
+      <c r="BN2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BO2" s="5" t="s">
+      <c r="BO2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BP2" s="5" t="s">
+      <c r="BP2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BQ2" s="5" t="s">
+      <c r="BQ2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BR2" s="5" t="s">
+      <c r="BR2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BS2" s="5" t="s">
+      <c r="BS2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BT2" s="5" t="s">
+      <c r="BT2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BU2" s="5" t="s">
+      <c r="BU2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BV2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BW2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BX2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="BY2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CA2" s="2" t="s">
+      <c r="CA2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CB2" s="2" t="s">
+      <c r="CB2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CC2" s="2" t="s">
+      <c r="CC2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CD2" s="2" t="s">
+      <c r="CD2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CE2" s="2" t="s">
+      <c r="CE2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CF2" s="2" t="s">
+      <c r="CF2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CG2" s="2" t="s">
+      <c r="CG2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CH2" s="2" t="s">
+      <c r="CH2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CI2" s="2" t="s">
+      <c r="CI2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CJ2" s="2" t="s">
+      <c r="CJ2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CK2" s="2" t="s">
+      <c r="CK2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CL2" s="2" t="s">
+      <c r="CL2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CM2" s="2" t="s">
+      <c r="CM2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CN2" s="2" t="s">
+      <c r="CN2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CO2" s="2" t="s">
+      <c r="CO2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CP2" s="2" t="s">
+      <c r="CP2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CQ2" s="2" t="s">
+      <c r="CQ2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CR2" s="2" t="s">
+      <c r="CR2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CS2" s="2" t="s">
+      <c r="CS2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CT2" s="2" t="s">
+      <c r="CT2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CU2" s="2" t="s">
+      <c r="CU2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CV2" s="2" t="s">
+      <c r="CV2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="CW2" s="2" t="s">
+      <c r="CW2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="CX2" s="2" t="s">
+      <c r="CX2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="CY2" s="2" t="s">
+      <c r="CY2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="CZ2" s="2" t="s">
+      <c r="CZ2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DA2" s="2" t="s">
+      <c r="DA2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DB2" s="2" t="s">
+      <c r="DB2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DC2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DD2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DE2" s="2" t="s">
+      <c r="DE2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DF2" s="2" t="s">
+      <c r="DF2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DG2" s="2" t="s">
+      <c r="DG2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="DH2" s="8" t="s">
+      <c r="DH2" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="DI2" s="8" t="s">
+      <c r="DI2" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="DJ2" s="8" t="s">
+      <c r="DJ2" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="DK2" s="8" t="s">
+      <c r="DK2" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="DL2" s="8" t="s">
+      <c r="DL2" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="DM2" s="8" t="s">
+      <c r="DM2" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="DN2" s="8" t="s">
+      <c r="DN2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="DO2" s="8" t="s">
+      <c r="DO2" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="DP2" s="8" t="s">
+      <c r="DP2" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="DQ2" s="8" t="s">
+      <c r="DQ2" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="DR2" s="8" t="s">
+      <c r="DR2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="DS2" s="8" t="s">
+      <c r="DS2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="DT2" s="8" t="s">
+      <c r="DT2" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="DU2" s="8" t="s">
+      <c r="DU2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="DV2" s="8" t="s">
+      <c r="DV2" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="DW2" s="8" t="s">
+      <c r="DW2" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="DX2" s="8" t="s">
+      <c r="DX2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="DY2" s="7" t="s">
+      <c r="DY2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="DZ2" s="7" t="s">
+      <c r="DZ2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="EA2" s="7" t="s">
+      <c r="EA2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="EB2" s="7" t="s">
+      <c r="EB2" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="EC2" s="7" t="s">
+      <c r="EC2" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="ED2" s="7" t="s">
+      <c r="ED2" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="EE2" s="7" t="s">
+      <c r="EE2" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="EF2" s="7" t="s">
+      <c r="EF2" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="16" spans="1:136" thickBot="1">
-      <c r="A3" s="9" t="s">
+    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="15" spans="1:136" thickBot="1">
+      <c r="A3" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="U3" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="V3" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="X3" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="Y3" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="Z3" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AA3" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AB3" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AC3" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="AE3" s="11" t="s">
+      <c r="AE3" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="AF3" s="11" t="s">
+      <c r="AF3" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="AG3" s="11" t="s">
+      <c r="AG3" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="AH3" s="11" t="s">
+      <c r="AH3" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AI3" s="11" t="s">
+      <c r="AI3" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="AJ3" s="11" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="AK3" s="11" t="s">
+      <c r="AK3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="AL3" s="11" t="s">
+      <c r="AL3" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="AM3" s="11" t="s">
+      <c r="AM3" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="AN3" s="11" t="s">
+      <c r="AN3" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="AO3" s="11" t="s">
+      <c r="AO3" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AP3" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="AR3" s="11" t="s">
+      <c r="AR3" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="AS3" s="11" t="s">
+      <c r="AS3" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="AT3" s="11" t="s">
+      <c r="AT3" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="AU3" s="11" t="s">
+      <c r="AU3" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="AV3" s="11" t="s">
+      <c r="AV3" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="AW3" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="AX3" s="11" t="s">
+      <c r="AX3" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="AY3" s="11" t="s">
+      <c r="AY3" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="AZ3" s="11" t="s">
+      <c r="AZ3" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="BA3" s="11" t="s">
+      <c r="BA3" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="BB3" s="11" t="s">
+      <c r="BB3" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="BC3" s="11" t="s">
+      <c r="BC3" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="BD3" s="11" t="s">
+      <c r="BD3" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="BE3" s="11" t="s">
+      <c r="BE3" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="BF3" s="11" t="s">
+      <c r="BF3" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="BG3" s="11" t="s">
+      <c r="BG3" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="BH3" s="11" t="s">
+      <c r="BH3" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="BI3" s="11" t="s">
+      <c r="BI3" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="BJ3" s="11" t="s">
+      <c r="BJ3" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="BK3" s="11" t="s">
+      <c r="BK3" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="BL3" s="11" t="s">
+      <c r="BL3" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="BM3" s="11" t="s">
+      <c r="BM3" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="BN3" s="11" t="s">
+      <c r="BN3" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="BO3" s="11" t="s">
+      <c r="BO3" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="BP3" s="11" t="s">
+      <c r="BP3" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="BQ3" s="11" t="s">
+      <c r="BQ3" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="BR3" s="11" t="s">
+      <c r="BR3" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="BS3" s="11" t="s">
+      <c r="BS3" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="BT3" s="11" t="s">
+      <c r="BT3" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="BU3" s="11" t="s">
+      <c r="BU3" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="BV3" s="12" t="s">
+      <c r="BV3" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="BW3" s="12" t="s">
+      <c r="BW3" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="BX3" s="12" t="s">
+      <c r="BX3" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="BY3" s="12" t="s">
+      <c r="BY3" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="BZ3" s="13" t="s">
+      <c r="BZ3" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="CA3" s="13" t="s">
+      <c r="CA3" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="CB3" s="13" t="s">
+      <c r="CB3" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="CC3" s="13" t="s">
+      <c r="CC3" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="CD3" s="13" t="s">
+      <c r="CD3" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="CE3" s="13" t="s">
+      <c r="CE3" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="CF3" s="13" t="s">
+      <c r="CF3" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="CG3" s="13" t="s">
+      <c r="CG3" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="CH3" s="13" t="s">
+      <c r="CH3" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="CI3" s="13" t="s">
+      <c r="CI3" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="CJ3" s="13" t="s">
+      <c r="CJ3" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="CK3" s="13" t="s">
+      <c r="CK3" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="CL3" s="13" t="s">
+      <c r="CL3" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="CM3" s="13" t="s">
+      <c r="CM3" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="CN3" s="13" t="s">
+      <c r="CN3" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="CO3" s="13" t="s">
+      <c r="CO3" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="CP3" s="13" t="s">
+      <c r="CP3" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="CQ3" s="13" t="s">
+      <c r="CQ3" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="CR3" s="13" t="s">
+      <c r="CR3" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="CS3" s="13" t="s">
+      <c r="CS3" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="CT3" s="13" t="s">
+      <c r="CT3" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="CU3" s="13" t="s">
+      <c r="CU3" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="CV3" s="13" t="s">
+      <c r="CV3" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="CW3" s="13" t="s">
+      <c r="CW3" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="CX3" s="13" t="s">
+      <c r="CX3" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="CY3" s="13" t="s">
+      <c r="CY3" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="CZ3" s="13" t="s">
+      <c r="CZ3" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="DA3" s="13" t="s">
+      <c r="DA3" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="DB3" s="13" t="s">
+      <c r="DB3" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="DC3" s="13" t="s">
+      <c r="DC3" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="DD3" s="13" t="s">
+      <c r="DD3" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="DE3" s="13" t="s">
+      <c r="DE3" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="DF3" s="13" t="s">
+      <c r="DF3" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="DG3" s="13" t="s">
+      <c r="DG3" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="DH3" s="14" t="s">
+      <c r="DH3" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="DI3" s="14" t="s">
+      <c r="DI3" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="DJ3" s="14" t="s">
+      <c r="DJ3" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="DK3" s="14" t="s">
+      <c r="DK3" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="DL3" s="14" t="s">
+      <c r="DL3" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="DM3" s="14" t="s">
+      <c r="DM3" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="DN3" s="14" t="s">
+      <c r="DN3" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="DO3" s="14" t="s">
+      <c r="DO3" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="DP3" s="14" t="s">
+      <c r="DP3" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="DQ3" s="14" t="s">
+      <c r="DQ3" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="DR3" s="14" t="s">
+      <c r="DR3" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="DS3" s="14" t="s">
+      <c r="DS3" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="DT3" s="14" t="s">
+      <c r="DT3" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="DU3" s="14" t="s">
+      <c r="DU3" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="DV3" s="14" t="s">
+      <c r="DV3" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="DW3" s="14" t="s">
+      <c r="DW3" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="DX3" s="14" t="s">
+      <c r="DX3" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="DY3" s="15" t="s">
+      <c r="DY3" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="DZ3" s="15" t="s">
+      <c r="DZ3" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="EA3" s="15" t="s">
+      <c r="EA3" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="EB3" s="15" t="s">
+      <c r="EB3" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="EC3" s="15" t="s">
+      <c r="EC3" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="ED3" s="15" t="s">
+      <c r="ED3" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="EE3" s="15" t="s">
+      <c r="EE3" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="EF3" s="15" t="s">
+      <c r="EF3" s="14" t="s">
         <v>272</v>
       </c>
     </row>
@@ -2323,7 +2336,7 @@
       <c r="H4" t="s">
         <v>277</v>
       </c>
-      <c r="I4" s="17" t="n">
+      <c r="I4" s="16" t="n">
         <v>43465</v>
       </c>
       <c r="K4" t="s">
@@ -2371,7 +2384,7 @@
       <c r="BJ4" t="n">
         <v>-123.3706457</v>
       </c>
-      <c r="BV4" s="17" t="n">
+      <c r="BV4" s="16" t="n">
         <v>43465</v>
       </c>
       <c r="BX4" t="s">
@@ -2415,7 +2428,7 @@
       <c r="H5" t="s">
         <v>277</v>
       </c>
-      <c r="I5" s="17" t="n">
+      <c r="I5" s="16" t="n">
         <v>43465</v>
       </c>
       <c r="K5" t="s">
@@ -2463,7 +2476,7 @@
       <c r="BJ5" t="n">
         <v>-123.3688604</v>
       </c>
-      <c r="BV5" s="17" t="n">
+      <c r="BV5" s="16" t="n">
         <v>43465</v>
       </c>
       <c r="BX5" t="s">
@@ -2533,13 +2546,7 @@
         <v>306</v>
       </c>
       <c r="B2" t="n">
-        <v>2430</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4829</v>
-      </c>
-      <c r="D2" t="n">
-        <v>5698</v>
+        <v>6168</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2547,36 +2554,48 @@
         <v>307</v>
       </c>
       <c r="B3" t="n">
-        <v>2767</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4659</v>
+        <v>6755</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>308</v>
       </c>
-      <c r="B4" t="n">
-        <v>6168</v>
-      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>309</v>
       </c>
       <c r="B5" t="n">
-        <v>6755</v>
+        <v>2430</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4829</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5698</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>310</v>
       </c>
+      <c r="B6" t="n">
+        <v>2767</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4659</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>311</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6755</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4659</v>
       </c>
     </row>
   </sheetData>
@@ -2608,18 +2627,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="B2" t="n">
-        <v>98675</v>
+        <v>98672</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="B3" t="n">
-        <v>98672</v>
+        <v>98675</v>
       </c>
     </row>
   </sheetData>
@@ -2773,6 +2792,9 @@
       </c>
     </row>
     <row r="2" spans="1:43">
+      <c r="A2" t="s">
+        <v>315</v>
+      </c>
       <c r="B2" t="n">
         <v>15</v>
       </c>
@@ -2806,7 +2828,37 @@
     </row>
     <row r="3" spans="1:43">
       <c r="A3" t="s">
-        <v>315</v>
+        <v>316</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" t="s">
+        <v>284</v>
+      </c>
+      <c r="I3" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>286</v>
+      </c>
+      <c r="T3" t="s">
+        <v>300</v>
+      </c>
+      <c r="V3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>48.419957</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>-123.3688604</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2828,9 +2880,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
@@ -2848,80 +2900,110 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>317</v>
+      </c>
       <c r="C2" t="s">
         <v>277</v>
       </c>
-      <c r="D2" s="25" t="n">
+      <c r="D2" s="26" t="n">
         <v>43465</v>
       </c>
       <c r="F2" t="s">
         <v>278</v>
       </c>
       <c r="G2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" t="s">
         <v>280</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>281</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" s="26" t="n">
+        <v>43465</v>
+      </c>
+      <c r="F3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" t="s">
         <v>298</v>
+      </c>
+      <c r="H3" t="s">
+        <v>280</v>
+      </c>
+      <c r="K3" t="s">
+        <v>281</v>
+      </c>
+      <c r="X3" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Update existing record functionality
</commit_message>
<xml_diff>
--- a/bulk_import_tool/IMM import template - test.xlsx
+++ b/bulk_import_tool/IMM import template - test.xlsx
@@ -4,21 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7860" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="IMM_template" sheetId="1" r:id="rId1"/>
-    <sheet name="Event" sheetId="2" r:id="rId2"/>
-    <sheet name="Site" sheetId="3" r:id="rId3"/>
-    <sheet name="Taxon" sheetId="4" r:id="rId4"/>
-    <sheet name="Person" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="309">
   <si>
     <t>Catalogue</t>
   </si>
@@ -945,45 +941,12 @@
   </si>
   <si>
     <t>Henry Choong; Heidi Gartner</t>
-  </si>
-  <si>
-    <t>Taxon</t>
-  </si>
-  <si>
-    <t>Taxon_ids</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Person_ids</t>
-  </si>
-  <si>
-    <t>Heidi Gartner</t>
-  </si>
-  <si>
-    <t>Hugh MacIntosh</t>
-  </si>
-  <si>
-    <t>Meg Sugrue</t>
-  </si>
-  <si>
-    <t>Henry Choong</t>
-  </si>
-  <si>
-    <t>Evan Harley</t>
-  </si>
-  <si>
-    <t>David Stewart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1072,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1093,7 +1056,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1419,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EF5"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Z5" sqref="Z5"/>
     </sheetView>
@@ -1477,156 +1439,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:136" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="23" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20"/>
-      <c r="BC1" s="20"/>
-      <c r="BD1" s="20"/>
-      <c r="BE1" s="20"/>
-      <c r="BF1" s="20"/>
-      <c r="BG1" s="20"/>
-      <c r="BH1" s="20"/>
-      <c r="BI1" s="20"/>
-      <c r="BJ1" s="20"/>
-      <c r="BK1" s="20"/>
-      <c r="BL1" s="20"/>
-      <c r="BM1" s="20"/>
-      <c r="BN1" s="20"/>
-      <c r="BO1" s="20"/>
-      <c r="BP1" s="20"/>
-      <c r="BQ1" s="20"/>
-      <c r="BR1" s="20"/>
-      <c r="BS1" s="20"/>
-      <c r="BT1" s="20"/>
-      <c r="BU1" s="20"/>
-      <c r="BV1" s="24" t="s">
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="19"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
+      <c r="BG1" s="19"/>
+      <c r="BH1" s="19"/>
+      <c r="BI1" s="19"/>
+      <c r="BJ1" s="19"/>
+      <c r="BK1" s="19"/>
+      <c r="BL1" s="19"/>
+      <c r="BM1" s="19"/>
+      <c r="BN1" s="19"/>
+      <c r="BO1" s="19"/>
+      <c r="BP1" s="19"/>
+      <c r="BQ1" s="19"/>
+      <c r="BR1" s="19"/>
+      <c r="BS1" s="19"/>
+      <c r="BT1" s="19"/>
+      <c r="BU1" s="19"/>
+      <c r="BV1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="BW1" s="20"/>
-      <c r="BX1" s="20"/>
-      <c r="BY1" s="20"/>
-      <c r="BZ1" s="25" t="s">
+      <c r="BW1" s="19"/>
+      <c r="BX1" s="19"/>
+      <c r="BY1" s="19"/>
+      <c r="BZ1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="CA1" s="20"/>
-      <c r="CB1" s="20"/>
-      <c r="CC1" s="20"/>
-      <c r="CD1" s="20"/>
-      <c r="CE1" s="20"/>
-      <c r="CF1" s="20"/>
-      <c r="CG1" s="20"/>
-      <c r="CH1" s="20"/>
-      <c r="CI1" s="20"/>
-      <c r="CJ1" s="20"/>
-      <c r="CK1" s="20"/>
-      <c r="CL1" s="20"/>
-      <c r="CM1" s="20"/>
-      <c r="CN1" s="20"/>
-      <c r="CO1" s="20"/>
-      <c r="CP1" s="20"/>
-      <c r="CQ1" s="20"/>
-      <c r="CR1" s="20"/>
-      <c r="CS1" s="20"/>
-      <c r="CT1" s="20"/>
-      <c r="CU1" s="20"/>
-      <c r="CV1" s="20"/>
-      <c r="CW1" s="20"/>
-      <c r="CX1" s="20"/>
-      <c r="CY1" s="20"/>
-      <c r="CZ1" s="20"/>
-      <c r="DA1" s="20"/>
-      <c r="DB1" s="20"/>
-      <c r="DC1" s="20"/>
-      <c r="DD1" s="20"/>
-      <c r="DE1" s="20"/>
-      <c r="DF1" s="20"/>
-      <c r="DG1" s="20"/>
-      <c r="DH1" s="26" t="s">
+      <c r="CA1" s="19"/>
+      <c r="CB1" s="19"/>
+      <c r="CC1" s="19"/>
+      <c r="CD1" s="19"/>
+      <c r="CE1" s="19"/>
+      <c r="CF1" s="19"/>
+      <c r="CG1" s="19"/>
+      <c r="CH1" s="19"/>
+      <c r="CI1" s="19"/>
+      <c r="CJ1" s="19"/>
+      <c r="CK1" s="19"/>
+      <c r="CL1" s="19"/>
+      <c r="CM1" s="19"/>
+      <c r="CN1" s="19"/>
+      <c r="CO1" s="19"/>
+      <c r="CP1" s="19"/>
+      <c r="CQ1" s="19"/>
+      <c r="CR1" s="19"/>
+      <c r="CS1" s="19"/>
+      <c r="CT1" s="19"/>
+      <c r="CU1" s="19"/>
+      <c r="CV1" s="19"/>
+      <c r="CW1" s="19"/>
+      <c r="CX1" s="19"/>
+      <c r="CY1" s="19"/>
+      <c r="CZ1" s="19"/>
+      <c r="DA1" s="19"/>
+      <c r="DB1" s="19"/>
+      <c r="DC1" s="19"/>
+      <c r="DD1" s="19"/>
+      <c r="DE1" s="19"/>
+      <c r="DF1" s="19"/>
+      <c r="DG1" s="19"/>
+      <c r="DH1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="DI1" s="20"/>
-      <c r="DJ1" s="20"/>
-      <c r="DK1" s="20"/>
-      <c r="DL1" s="20"/>
-      <c r="DM1" s="20"/>
-      <c r="DN1" s="20"/>
-      <c r="DO1" s="20"/>
-      <c r="DP1" s="20"/>
-      <c r="DQ1" s="20"/>
-      <c r="DR1" s="20"/>
-      <c r="DS1" s="20"/>
-      <c r="DT1" s="20"/>
-      <c r="DU1" s="20"/>
-      <c r="DV1" s="20"/>
-      <c r="DW1" s="20"/>
-      <c r="DX1" s="20"/>
-      <c r="DY1" s="19" t="s">
+      <c r="DI1" s="19"/>
+      <c r="DJ1" s="19"/>
+      <c r="DK1" s="19"/>
+      <c r="DL1" s="19"/>
+      <c r="DM1" s="19"/>
+      <c r="DN1" s="19"/>
+      <c r="DO1" s="19"/>
+      <c r="DP1" s="19"/>
+      <c r="DQ1" s="19"/>
+      <c r="DR1" s="19"/>
+      <c r="DS1" s="19"/>
+      <c r="DT1" s="19"/>
+      <c r="DU1" s="19"/>
+      <c r="DV1" s="19"/>
+      <c r="DW1" s="19"/>
+      <c r="DX1" s="19"/>
+      <c r="DY1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="DZ1" s="20"/>
-      <c r="EA1" s="20"/>
-      <c r="EB1" s="20"/>
-      <c r="EC1" s="20"/>
-      <c r="ED1" s="20"/>
-      <c r="EE1" s="20"/>
-      <c r="EF1" s="20"/>
+      <c r="DZ1" s="19"/>
+      <c r="EA1" s="19"/>
+      <c r="EB1" s="19"/>
+      <c r="EC1" s="19"/>
+      <c r="ED1" s="19"/>
+      <c r="EE1" s="19"/>
+      <c r="EF1" s="19"/>
     </row>
     <row r="2" spans="1:136" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2657,486 +2619,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X3"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D2" s="18">
-        <v>43465</v>
-      </c>
-      <c r="F2" t="s">
-        <v>279</v>
-      </c>
-      <c r="G2" t="s">
-        <v>281</v>
-      </c>
-      <c r="H2" t="s">
-        <v>282</v>
-      </c>
-      <c r="K2" t="s">
-        <v>283</v>
-      </c>
-      <c r="X2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>301</v>
-      </c>
-      <c r="C3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D3" s="18">
-        <v>43465</v>
-      </c>
-      <c r="F3" t="s">
-        <v>279</v>
-      </c>
-      <c r="G3" t="s">
-        <v>302</v>
-      </c>
-      <c r="H3" t="s">
-        <v>282</v>
-      </c>
-      <c r="K3" t="s">
-        <v>283</v>
-      </c>
-      <c r="X3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" t="s">
-        <v>10</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>285</v>
-      </c>
-      <c r="H2" t="s">
-        <v>286</v>
-      </c>
-      <c r="I2" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>288</v>
-      </c>
-      <c r="T2" t="s">
-        <v>289</v>
-      </c>
-      <c r="U2" t="s">
-        <v>290</v>
-      </c>
-      <c r="W2" t="s">
-        <v>291</v>
-      </c>
-      <c r="AE2">
-        <v>48.419603000000002</v>
-      </c>
-      <c r="AG2">
-        <v>-123.3706457</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>285</v>
-      </c>
-      <c r="H3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I3" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>288</v>
-      </c>
-      <c r="T3" t="s">
-        <v>304</v>
-      </c>
-      <c r="U3" t="s">
-        <v>305</v>
-      </c>
-      <c r="W3" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE3">
-        <v>48.419956999999997</v>
-      </c>
-      <c r="AG3">
-        <v>-123.3688604</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B2">
-        <v>98672</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B3">
-        <v>98675</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>313</v>
-      </c>
-      <c r="B2">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B3">
-        <v>6755</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>315</v>
-      </c>
-      <c r="B4">
-        <v>16213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B5">
-        <v>2767</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>317</v>
-      </c>
-      <c r="B6">
-        <v>6168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B7">
-        <v>14477</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Human History Integration complete
</commit_message>
<xml_diff>
--- a/bulk_import_tool/IMM import template - test.xlsx
+++ b/bulk_import_tool/IMM import template - test.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7860" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7860"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IMM_template" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Taxon" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Event" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Site" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="IMM_template" sheetId="1" r:id="rId1"/>
+    <sheet name="Event" sheetId="2" r:id="rId2"/>
+    <sheet name="Organization" sheetId="3" r:id="rId3"/>
+    <sheet name="Person" sheetId="4" r:id="rId4"/>
+    <sheet name="Taxon" sheetId="5" r:id="rId5"/>
+    <sheet name="Site" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="330">
   <si>
     <t>Catalogue</t>
   </si>
@@ -431,6 +432,9 @@
     <t>Measurement Comment</t>
   </si>
   <si>
+    <t>Previous Number</t>
+  </si>
+  <si>
     <t>Item.registration_num</t>
   </si>
   <si>
@@ -503,6 +507,9 @@
     <t>CollectionEvent.vessel_name</t>
   </si>
   <si>
+    <t>person_id</t>
+  </si>
+  <si>
     <t>Person.search_name</t>
   </si>
   <si>
@@ -662,6 +669,9 @@
     <t>Taxonomy.notes</t>
   </si>
   <si>
+    <t>taxon_id</t>
+  </si>
+  <si>
     <t>Taxon.term</t>
   </si>
   <si>
@@ -839,6 +849,9 @@
     <t>Measurement.comment</t>
   </si>
   <si>
+    <t>OtherNumber.identifier</t>
+  </si>
+  <si>
     <t>TEST_CN_01</t>
   </si>
   <si>
@@ -857,7 +870,7 @@
     <t>INV</t>
   </si>
   <si>
-    <t>VE18219</t>
+    <t>VE18341</t>
   </si>
   <si>
     <t>EV1</t>
@@ -869,9 +882,15 @@
     <t>Winter</t>
   </si>
   <si>
+    <t>6755; 6168</t>
+  </si>
+  <si>
     <t>Hugh MacIntosh; Evan Harley</t>
   </si>
   <si>
+    <t>Washington Department of Fish and Wildlife</t>
+  </si>
+  <si>
     <t>m</t>
   </si>
   <si>
@@ -884,7 +903,7 @@
     <t>British Columbia</t>
   </si>
   <si>
-    <t>VS102279</t>
+    <t>VS102391</t>
   </si>
   <si>
     <t>Fannin tower, 2nd floor</t>
@@ -920,16 +939,19 @@
     <t>Test item 2</t>
   </si>
   <si>
-    <t>VE18220</t>
+    <t>VE18342</t>
   </si>
   <si>
     <t>EV2</t>
   </si>
   <si>
+    <t>16213; NEW?</t>
+  </si>
+  <si>
     <t>Meg Sugrue; David Stewart</t>
   </si>
   <si>
-    <t>VS102280</t>
+    <t>VS102392</t>
   </si>
   <si>
     <t>Clifford Carl Hall</t>
@@ -938,72 +960,84 @@
     <t>Victoria: RBCM Exhibits building</t>
   </si>
   <si>
+    <t>NEW?</t>
+  </si>
+  <si>
     <t>Cancer magister</t>
   </si>
   <si>
     <t>Henry Choong; Heidi Gartner</t>
   </si>
   <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Organization_ids</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Person_ids</t>
+  </si>
+  <si>
+    <t>Hugh MacIntosh</t>
+  </si>
+  <si>
+    <t>Meg Sugrue</t>
+  </si>
+  <si>
+    <t>Henry Choong</t>
+  </si>
+  <si>
+    <t>Heidi Gartner</t>
+  </si>
+  <si>
+    <t>David Stewart</t>
+  </si>
+  <si>
+    <t>Evan Harley</t>
+  </si>
+  <si>
     <t>Taxon</t>
   </si>
   <si>
     <t>Taxon_ids</t>
   </si>
   <si>
-    <t>NEW?</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Person_ids</t>
-  </si>
-  <si>
-    <t>Hugh MacIntosh</t>
-  </si>
-  <si>
-    <t>Heidi Gartner</t>
-  </si>
-  <si>
-    <t>David Stewart</t>
-  </si>
-  <si>
-    <t>Meg Sugrue</t>
-  </si>
-  <si>
-    <t>Evan Harley</t>
-  </si>
-  <si>
-    <t>Henry Choong</t>
+    <t>08/01/2002</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1016,31 +1050,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999755851924192"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.1499984740745262"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,43 +1104,55 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1396,82 +1442,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:EH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:EM5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A4" ySplit="3"/>
-      <selection activeCell="AR4" pane="bottomLeft" sqref="AR4"/>
+    <sheetView tabSelected="1" topLeftCell="DM1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="EA11" sqref="EA11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="21.42578125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="19.42578125"/>
-    <col bestFit="1" customWidth="1" max="4" min="3" width="19.5703125"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="40.42578125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="20.28515625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="16"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="34"/>
-    <col customWidth="1" max="9" min="9" width="16.42578125"/>
-    <col customWidth="1" max="11" min="10" width="17.7109375"/>
-    <col customWidth="1" max="12" min="12" width="17.140625"/>
-    <col customWidth="1" max="13" min="13" width="17.42578125"/>
-    <col customWidth="1" max="14" min="14" width="19.28515625"/>
-    <col customWidth="1" max="15" min="15" width="18"/>
-    <col customWidth="1" max="16" min="16" width="19.42578125"/>
-    <col customWidth="1" max="17" min="17" width="16.85546875"/>
-    <col customWidth="1" max="18" min="18" width="17"/>
-    <col customWidth="1" max="19" min="19" width="17.42578125"/>
-    <col customWidth="1" max="20" min="20" width="17.5703125"/>
-    <col customWidth="1" max="21" min="21" width="27.5703125"/>
-    <col customWidth="1" max="22" min="22" width="17.7109375"/>
-    <col bestFit="1" customWidth="1" max="23" min="23" width="27"/>
-    <col customWidth="1" max="24" min="24" width="18.140625"/>
-    <col customWidth="1" max="28" min="25" width="17.7109375"/>
-    <col customWidth="1" max="44" min="29" width="16.7109375"/>
-    <col customWidth="1" max="45" min="45" width="24.5703125"/>
-    <col customWidth="1" max="62" min="46" width="16.7109375"/>
-    <col customWidth="1" max="63" min="63" width="23.5703125"/>
-    <col customWidth="1" max="64" min="64" width="18.5703125"/>
-    <col customWidth="1" max="69" min="65" width="16.7109375"/>
-    <col customWidth="1" max="70" min="70" width="18.5703125"/>
-    <col customWidth="1" max="71" min="71" width="16.7109375"/>
-    <col customWidth="1" max="72" min="72" width="18.7109375"/>
-    <col customWidth="1" max="73" min="73" width="17"/>
-    <col customWidth="1" max="74" min="74" width="20"/>
-    <col customWidth="1" max="75" min="75" width="16.7109375"/>
-    <col customWidth="1" max="107" min="76" width="18.7109375"/>
-    <col customWidth="1" max="108" min="108" width="20.28515625"/>
-    <col customWidth="1" max="123" min="109" width="17.7109375"/>
-    <col customWidth="1" max="124" min="124" width="11.140625"/>
-    <col customWidth="1" max="125" min="125" width="13.42578125"/>
-    <col customWidth="1" max="126" min="126" width="15.85546875"/>
-    <col customWidth="1" max="127" min="127" width="10.7109375"/>
-    <col customWidth="1" max="128" min="128" width="20.28515625"/>
-    <col customWidth="1" max="129" min="129" width="19.85546875"/>
-    <col customWidth="1" max="130" min="130" width="22"/>
-    <col customWidth="1" max="131" min="131" width="25"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" customWidth="1"/>
+    <col min="21" max="21" width="27.5703125" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" customWidth="1"/>
+    <col min="25" max="27" width="17.7109375" customWidth="1"/>
+    <col min="28" max="43" width="16.7109375" customWidth="1"/>
+    <col min="44" max="44" width="24.5703125" customWidth="1"/>
+    <col min="45" max="61" width="16.7109375" customWidth="1"/>
+    <col min="62" max="62" width="23.5703125" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="68" width="16.7109375" customWidth="1"/>
+    <col min="69" max="69" width="18.5703125" customWidth="1"/>
+    <col min="70" max="70" width="16.7109375" customWidth="1"/>
+    <col min="71" max="71" width="18.7109375" customWidth="1"/>
+    <col min="72" max="72" width="17" customWidth="1"/>
+    <col min="73" max="73" width="20" customWidth="1"/>
+    <col min="74" max="74" width="16.7109375" customWidth="1"/>
+    <col min="75" max="105" width="18.7109375" customWidth="1"/>
+    <col min="106" max="106" width="20.28515625" customWidth="1"/>
+    <col min="107" max="122" width="17.7109375" customWidth="1"/>
+    <col min="123" max="123" width="11.140625" customWidth="1"/>
+    <col min="124" max="124" width="13.42578125" customWidth="1"/>
+    <col min="125" max="125" width="20.28515625" customWidth="1"/>
+    <col min="126" max="126" width="19.85546875" customWidth="1"/>
+    <col min="127" max="127" width="22" customWidth="1"/>
+    <col min="128" max="128" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="20" spans="1:138">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:143" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="20" t="n"/>
-      <c r="BP1" s="20" t="n"/>
-      <c r="BS1" s="20" t="n"/>
-      <c r="CL1" s="20" t="n"/>
-      <c r="DA1" s="20" t="n"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22"/>
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22"/>
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
+      <c r="CC1" s="22"/>
+      <c r="CD1" s="22"/>
+      <c r="CE1" s="22"/>
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="22"/>
+      <c r="CO1" s="22"/>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="22"/>
+      <c r="CT1" s="22"/>
+      <c r="CU1" s="22"/>
+      <c r="CV1" s="22"/>
+      <c r="CW1" s="22"/>
+      <c r="CX1" s="22"/>
+      <c r="CY1" s="22"/>
+      <c r="CZ1" s="22"/>
+      <c r="DA1" s="22"/>
+      <c r="DB1" s="22"/>
+      <c r="DC1" s="22"/>
+      <c r="DD1" s="22"/>
+      <c r="DE1" s="22"/>
+      <c r="DF1" s="22"/>
+      <c r="DG1" s="22"/>
+      <c r="DH1" s="22"/>
+      <c r="DI1" s="22"/>
+      <c r="DJ1" s="22"/>
+      <c r="EM1" s="19"/>
     </row>
-    <row customFormat="1" r="2" s="20" spans="1:138">
+    <row r="2" spans="1:143" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1544,1467 +1692,1554 @@
       <c r="X2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AU2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BH2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BI2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BM2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BO2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BO2" s="4" t="s">
+      <c r="BP2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BP2" s="4" t="s">
+      <c r="BQ2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BR2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BS2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="BT2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BU2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="BV2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BW2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BX2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BX2" s="3" t="s">
+      <c r="BY2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="BY2" s="3" t="s">
+      <c r="BZ2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="BZ2" s="3" t="s">
+      <c r="CB2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="CA2" s="3" t="s">
+      <c r="CC2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="CB2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CC2" s="1" t="s">
+      <c r="CF2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CD2" s="1" t="s">
+      <c r="CG2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CE2" s="1" t="s">
+      <c r="CH2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CF2" s="1" t="s">
+      <c r="CI2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CG2" s="1" t="s">
+      <c r="CJ2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CH2" s="1" t="s">
+      <c r="CK2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CI2" s="1" t="s">
+      <c r="CL2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CJ2" s="1" t="s">
+      <c r="CM2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CK2" s="1" t="s">
+      <c r="CN2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CL2" s="1" t="s">
+      <c r="CO2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CM2" s="1" t="s">
+      <c r="CP2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CN2" s="1" t="s">
+      <c r="CQ2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CO2" s="1" t="s">
+      <c r="CR2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CP2" s="1" t="s">
+      <c r="CS2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CQ2" s="1" t="s">
+      <c r="CT2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CR2" s="1" t="s">
+      <c r="CU2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CS2" s="1" t="s">
+      <c r="CV2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CT2" s="1" t="s">
+      <c r="CW2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CU2" s="1" t="s">
+      <c r="CX2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CV2" s="1" t="s">
+      <c r="CY2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CW2" s="1" t="s">
+      <c r="CZ2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CX2" s="1" t="s">
+      <c r="DA2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CY2" s="1" t="s">
+      <c r="DB2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CZ2" s="1" t="s">
+      <c r="DC2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DA2" s="1" t="s">
+      <c r="DD2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DB2" s="1" t="s">
+      <c r="DE2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DC2" s="1" t="s">
+      <c r="DF2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DD2" s="1" t="s">
+      <c r="DG2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DE2" s="1" t="s">
+      <c r="DH2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DF2" s="1" t="s">
+      <c r="DI2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DG2" s="1" t="s">
+      <c r="DJ2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DH2" s="1" t="s">
+      <c r="DK2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DI2" s="1" t="s">
+      <c r="DL2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DJ2" s="7" t="s">
+      <c r="DM2" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="DK2" s="7" t="s">
+      <c r="DN2" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="DL2" s="7" t="s">
+      <c r="DO2" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="DM2" s="7" t="s">
+      <c r="DP2" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="DN2" s="7" t="s">
+      <c r="DQ2" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="DO2" s="7" t="s">
+      <c r="DR2" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="DP2" s="7" t="s">
+      <c r="DT2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="DQ2" s="7" t="s">
+      <c r="DU2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="DR2" s="7" t="s">
+      <c r="DV2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="DS2" s="7" t="s">
+      <c r="DW2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="DT2" s="7" t="s">
+      <c r="DX2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="DU2" s="7" t="s">
+      <c r="DY2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="DV2" s="7" t="s">
+      <c r="DZ2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="DW2" s="7" t="s">
+      <c r="EA2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="DX2" s="7" t="s">
+      <c r="EB2" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="DY2" s="7" t="s">
+      <c r="EC2" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="DZ2" s="7" t="s">
+      <c r="ED2" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="EA2" s="6" t="s">
+      <c r="EE2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="EB2" s="6" t="s">
+      <c r="EF2" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="EC2" s="6" t="s">
+      <c r="EG2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="ED2" s="6" t="s">
+      <c r="EH2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="EE2" s="6" t="s">
+      <c r="EI2" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="EF2" s="6" t="s">
+      <c r="EJ2" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="EG2" s="6" t="s">
+      <c r="EK2" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="EH2" s="6" t="s">
+      <c r="EL2" s="19" t="s">
         <v>136</v>
       </c>
+      <c r="EM2" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="15" spans="1:138" thickBot="1">
-      <c r="A3" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="18" t="s">
+    <row r="3" spans="1:143" s="14" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="N3" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="O3" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="P3" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="Q3" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="R3" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="S3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="T3" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="U3" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="V3" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="W3" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="X3" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="Y3" t="s">
         <v>162</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="Z3" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AA3" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AB3" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="AD3" s="9" t="s">
+      <c r="AC3" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="AE3" s="9" t="s">
+      <c r="AD3" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="AF3" s="9" t="s">
+      <c r="AE3" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AF3" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AH3" s="10" t="s">
+      <c r="AG3" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="AI3" s="10" t="s">
+      <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="AJ3" s="10" t="s">
+      <c r="AI3" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="AK3" s="10" t="s">
+      <c r="AJ3" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="AL3" s="10" t="s">
+      <c r="AK3" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="AM3" s="10" t="s">
+      <c r="AL3" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="AN3" s="10" t="s">
+      <c r="AM3" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="AO3" s="10" t="s">
+      <c r="AN3" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="AP3" s="10" t="s">
+      <c r="AO3" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="AQ3" s="10" t="s">
+      <c r="AP3" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="AR3" s="10" t="s">
+      <c r="AQ3" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="AS3" s="10" t="s">
+      <c r="AR3" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="AT3" s="10" t="s">
+      <c r="AS3" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="AU3" s="10" t="s">
+      <c r="AT3" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="AV3" s="10" t="s">
+      <c r="AU3" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="AW3" s="10" t="s">
+      <c r="AV3" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="AX3" s="10" t="s">
+      <c r="AW3" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="AY3" s="10" t="s">
+      <c r="AX3" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="AZ3" s="10" t="s">
+      <c r="AY3" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="BA3" s="10" t="s">
+      <c r="AZ3" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="BB3" s="10" t="s">
+      <c r="BA3" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="BC3" s="10" t="s">
+      <c r="BB3" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="BD3" s="10" t="s">
+      <c r="BC3" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="BE3" s="10" t="s">
+      <c r="BD3" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="BF3" s="10" t="s">
+      <c r="BE3" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="BG3" s="10" t="s">
+      <c r="BF3" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="BH3" s="10" t="s">
+      <c r="BG3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="BI3" s="10" t="s">
+      <c r="BH3" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="BJ3" s="10" t="s">
+      <c r="BI3" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="BK3" s="10" t="s">
+      <c r="BJ3" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="BL3" s="10" t="s">
+      <c r="BK3" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="BM3" s="10" t="s">
+      <c r="BL3" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="BN3" s="10" t="s">
+      <c r="BM3" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="BO3" s="10" t="s">
+      <c r="BN3" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="BP3" s="10" t="s">
+      <c r="BO3" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="BQ3" s="10" t="s">
+      <c r="BP3" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="BR3" s="10" t="s">
+      <c r="BQ3" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="BS3" s="10" t="s">
+      <c r="BR3" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="BT3" s="10" t="s">
+      <c r="BS3" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="BU3" s="10" t="s">
+      <c r="BT3" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="BV3" s="10" t="s">
+      <c r="BU3" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="BW3" s="10" t="s">
+      <c r="BV3" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="BX3" s="11" t="s">
+      <c r="BW3" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="BY3" s="11" t="s">
+      <c r="BX3" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="BZ3" s="11" t="s">
+      <c r="BY3" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="CA3" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="CB3" s="12" t="s">
+      <c r="BZ3" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="CC3" s="12" t="s">
+      <c r="CA3" t="s">
         <v>216</v>
       </c>
-      <c r="CD3" s="12" t="s">
+      <c r="CB3" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="CE3" s="12" t="s">
+      <c r="CC3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>162</v>
+      </c>
+      <c r="CE3" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="CF3" s="12" t="s">
+      <c r="CF3" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="CG3" s="12" t="s">
+      <c r="CG3" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="CH3" s="12" t="s">
+      <c r="CH3" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="CI3" s="12" t="s">
+      <c r="CI3" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="CJ3" s="12" t="s">
+      <c r="CJ3" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="CK3" s="12" t="s">
+      <c r="CK3" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="CL3" s="12" t="s">
+      <c r="CL3" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="CM3" s="12" t="s">
+      <c r="CM3" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="CN3" s="12" t="s">
+      <c r="CN3" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="CO3" s="12" t="s">
+      <c r="CO3" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="CP3" s="12" t="s">
+      <c r="CP3" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="CQ3" s="12" t="s">
+      <c r="CQ3" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="CR3" s="12" t="s">
+      <c r="CR3" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="CS3" s="12" t="s">
+      <c r="CS3" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="CT3" s="12" t="s">
+      <c r="CT3" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="CU3" s="12" t="s">
+      <c r="CU3" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="CV3" s="12" t="s">
+      <c r="CV3" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="CW3" s="12" t="s">
+      <c r="CW3" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="CX3" s="12" t="s">
+      <c r="CX3" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="CY3" s="12" t="s">
+      <c r="CY3" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="CZ3" s="12" t="s">
+      <c r="CZ3" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="DA3" s="12" t="s">
+      <c r="DA3" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="DB3" s="12" t="s">
+      <c r="DB3" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="DC3" s="12" t="s">
+      <c r="DC3" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="DD3" s="12" t="s">
+      <c r="DD3" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="DE3" s="12" t="s">
+      <c r="DE3" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="DF3" s="12" t="s">
+      <c r="DF3" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="DG3" s="12" t="s">
+      <c r="DG3" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="DH3" s="12" t="s">
+      <c r="DH3" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="DI3" s="12" t="s">
+      <c r="DI3" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="DJ3" s="13" t="s">
+      <c r="DJ3" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="DK3" s="13" t="s">
+      <c r="DK3" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="DL3" s="13" t="s">
+      <c r="DL3" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="DM3" s="13" t="s">
+      <c r="DM3" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="DN3" s="13" t="s">
+      <c r="DN3" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="DO3" s="13" t="s">
+      <c r="DO3" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="DP3" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="DQ3" s="13" t="s">
+      <c r="DP3" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="DR3" s="13" t="s">
+      <c r="DQ3" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="DS3" s="13" t="s">
+      <c r="DR3" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="DT3" s="13" t="s">
+      <c r="DS3" t="s">
+        <v>162</v>
+      </c>
+      <c r="DT3" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="DU3" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="DU3" s="13" t="s">
+      <c r="DV3" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="DV3" s="13" t="s">
+      <c r="DW3" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="DW3" s="13" t="s">
+      <c r="DX3" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="DX3" s="13" t="s">
+      <c r="DY3" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="DY3" s="13" t="s">
+      <c r="DZ3" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="DZ3" s="13" t="s">
+      <c r="EA3" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="EA3" s="14" t="s">
+      <c r="EB3" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="EB3" s="14" t="s">
+      <c r="EC3" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="EC3" s="14" t="s">
+      <c r="ED3" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="ED3" s="14" t="s">
+      <c r="EE3" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="EE3" s="14" t="s">
+      <c r="EF3" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="EF3" s="14" t="s">
+      <c r="EG3" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="EG3" s="14" t="s">
+      <c r="EH3" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="EH3" s="14" t="s">
+      <c r="EI3" s="13" t="s">
         <v>272</v>
       </c>
+      <c r="EJ3" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="EK3" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="EL3" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="EM3" s="19" t="s">
+        <v>276</v>
+      </c>
     </row>
-    <row r="4" spans="1:138">
+    <row r="4" spans="1:143" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F4" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="J4" t="s">
-        <v>277</v>
-      </c>
-      <c r="K4" s="16" t="n">
+        <v>281</v>
+      </c>
+      <c r="K4" s="15">
         <v>43465</v>
       </c>
       <c r="M4" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="N4" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="O4" t="s">
+        <v>284</v>
+      </c>
+      <c r="P4" t="s">
+        <v>285</v>
+      </c>
+      <c r="S4" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AH4">
+        <v>15</v>
+      </c>
+      <c r="AI4">
+        <v>14</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>290</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>291</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>292</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>293</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>294</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>295</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>296</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>328</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>329</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>329</v>
+      </c>
+      <c r="BK4">
+        <v>48.419603000000002</v>
+      </c>
+      <c r="BM4">
+        <v>-123.3706457</v>
+      </c>
+      <c r="BY4" s="15">
+        <v>43465</v>
+      </c>
+      <c r="CA4">
+        <v>98672</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>297</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>288</v>
+      </c>
+      <c r="DN4" t="s">
+        <v>298</v>
+      </c>
+      <c r="DO4" t="s">
+        <v>299</v>
+      </c>
+      <c r="DR4" t="s">
+        <v>300</v>
+      </c>
+      <c r="DZ4">
+        <v>1</v>
+      </c>
+      <c r="EB4" t="s">
+        <v>301</v>
+      </c>
+      <c r="EC4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F5" t="s">
         <v>280</v>
       </c>
-      <c r="P4" t="s">
+      <c r="J5" t="s">
         <v>281</v>
       </c>
-      <c r="S4" t="s">
+      <c r="K5" s="15">
+        <v>43465</v>
+      </c>
+      <c r="M5" t="s">
         <v>282</v>
       </c>
-      <c r="Y4" t="s">
-        <v>283</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>15</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>14</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>284</v>
-      </c>
-      <c r="AM4" t="s">
+      <c r="N5" t="s">
+        <v>306</v>
+      </c>
+      <c r="O5" t="s">
+        <v>307</v>
+      </c>
+      <c r="P5" t="s">
         <v>285</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="S5" t="s">
         <v>286</v>
       </c>
-      <c r="AV4" t="s">
-        <v>287</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>288</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>289</v>
-      </c>
-      <c r="BB4" t="s">
+      <c r="Y5" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AH5">
+        <v>5</v>
+      </c>
+      <c r="AI5">
+        <v>4</v>
+      </c>
+      <c r="AK5" t="s">
         <v>290</v>
       </c>
-      <c r="BJ4" t="n">
-        <v>48.419603</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>-123.3706457</v>
-      </c>
-      <c r="BX4" s="16" t="n">
+      <c r="AN5" t="s">
+        <v>291</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>292</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>293</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>310</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>311</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>312</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>328</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>329</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>329</v>
+      </c>
+      <c r="BK5">
+        <v>48.419956999999997</v>
+      </c>
+      <c r="BM5">
+        <v>-123.3688604</v>
+      </c>
+      <c r="BY5" s="15">
         <v>43465</v>
       </c>
-      <c r="BZ4" t="s">
-        <v>291</v>
-      </c>
-      <c r="CA4" t="s">
-        <v>283</v>
-      </c>
-      <c r="DK4" t="s">
-        <v>292</v>
-      </c>
-      <c r="DL4" t="s">
-        <v>293</v>
-      </c>
-      <c r="DO4" t="s">
-        <v>294</v>
-      </c>
-      <c r="DV4" t="n">
+      <c r="CA5" t="s">
+        <v>313</v>
+      </c>
+      <c r="CB5" t="s">
+        <v>314</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>315</v>
+      </c>
+      <c r="DN5" t="s">
+        <v>298</v>
+      </c>
+      <c r="DO5" t="s">
+        <v>299</v>
+      </c>
+      <c r="DR5" t="s">
+        <v>300</v>
+      </c>
+      <c r="DZ5">
         <v>1</v>
       </c>
-      <c r="DX4" t="s">
-        <v>295</v>
-      </c>
-      <c r="DY4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="5" spans="1:138">
-      <c r="B5" t="s">
-        <v>297</v>
-      </c>
-      <c r="C5" t="s">
-        <v>298</v>
-      </c>
-      <c r="D5" t="s">
-        <v>299</v>
-      </c>
-      <c r="F5" t="s">
-        <v>276</v>
-      </c>
-      <c r="J5" t="s">
-        <v>277</v>
-      </c>
-      <c r="K5" s="16" t="n">
-        <v>43465</v>
-      </c>
-      <c r="M5" t="s">
-        <v>278</v>
-      </c>
-      <c r="N5" t="s">
-        <v>300</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="EB5" t="s">
         <v>301</v>
       </c>
-      <c r="P5" t="s">
-        <v>281</v>
-      </c>
-      <c r="S5" t="s">
-        <v>282</v>
-      </c>
-      <c r="Y5" t="s">
+      <c r="EC5" t="s">
         <v>302</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>284</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>286</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>303</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>304</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>305</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>48.419957</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>-123.3688604</v>
-      </c>
-      <c r="BX5" s="16" t="n">
-        <v>43465</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>306</v>
-      </c>
-      <c r="CA5" t="s">
-        <v>307</v>
-      </c>
-      <c r="DK5" t="s">
-        <v>292</v>
-      </c>
-      <c r="DL5" t="s">
-        <v>293</v>
-      </c>
-      <c r="DO5" t="s">
-        <v>294</v>
-      </c>
-      <c r="DV5" t="n">
-        <v>1</v>
-      </c>
-      <c r="DX5" t="s">
-        <v>295</v>
-      </c>
-      <c r="DY5" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="CL1:CZ1"/>
-    <mergeCell ref="DA1:DF1"/>
+    <mergeCell ref="DE1:DJ1"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:Y1"/>
-    <mergeCell ref="Z1:BO1"/>
-    <mergeCell ref="BP1:BR1"/>
-    <mergeCell ref="BS1:CK1"/>
+    <mergeCell ref="I1:Z1"/>
+    <mergeCell ref="AA1:BP1"/>
+    <mergeCell ref="BQ1:BS1"/>
+    <mergeCell ref="BT1:CO1"/>
+    <mergeCell ref="CP1:DD1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>308</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>309</v>
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2" t="n">
-        <v>98672</v>
+        <v>283</v>
+      </c>
+      <c r="C2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="20">
+        <v>43465</v>
+      </c>
+      <c r="F2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I2" t="s">
+        <v>285</v>
+      </c>
+      <c r="L2" t="s">
+        <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>306</v>
       </c>
-      <c r="B3" t="s">
-        <v>310</v>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="20">
+        <v>43465</v>
+      </c>
+      <c r="F3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I3" t="s">
+        <v>285</v>
+      </c>
+      <c r="L3" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" t="s">
-        <v>33</v>
+        <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D2" s="22" t="n">
-        <v>43465</v>
-      </c>
-      <c r="F2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G2" t="s">
-        <v>279</v>
-      </c>
-      <c r="H2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I2" t="s">
-        <v>281</v>
-      </c>
-      <c r="L2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
-        <v>300</v>
-      </c>
-      <c r="C3" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="22" t="n">
-        <v>43465</v>
-      </c>
-      <c r="F3" t="s">
-        <v>278</v>
-      </c>
-      <c r="G3" t="s">
-        <v>300</v>
-      </c>
-      <c r="H3" t="s">
-        <v>301</v>
-      </c>
-      <c r="I3" t="s">
-        <v>281</v>
-      </c>
-      <c r="L3" t="s">
-        <v>282</v>
+        <v>289</v>
+      </c>
+      <c r="B2">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2">
+        <v>6755</v>
+      </c>
+      <c r="C2">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3">
+        <v>16213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>322</v>
+      </c>
+      <c r="B4">
+        <v>2767</v>
+      </c>
+      <c r="C4">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B5">
+        <v>2430</v>
+      </c>
+      <c r="C5">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B6" t="s">
         <v>313</v>
       </c>
-      <c r="B2" t="n">
-        <v>6755</v>
+      <c r="C6">
+        <v>4829</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2430</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4829</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>315</v>
-      </c>
-      <c r="B4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B5" t="n">
-        <v>16213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>317</v>
-      </c>
-      <c r="B6" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B7">
         <v>6168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2767</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2">
+        <v>98672</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="26" max="26" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="J1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="M1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="N1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="O1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="P1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="Q1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="R1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="S1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="T1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="V1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="W1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="X1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="Y1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Z1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="AA1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="AB1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="AC1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AD1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AE1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AF1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="AG1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AH1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AI1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AJ1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AK1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AL1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AM1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AN1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AO1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AP1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AQ1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AR1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" t="n">
+        <v>294</v>
+      </c>
+      <c r="B2">
         <v>15</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="H2" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="I2" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="Q2" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="T2" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="U2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="W2" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>329</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE2">
+        <v>48.419603000000002</v>
+      </c>
+      <c r="AG2">
+        <v>-123.3706457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
         <v>290</v>
       </c>
-      <c r="AE2" t="n">
-        <v>48.419603</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>-123.3706457</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44">
-      <c r="A3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>284</v>
-      </c>
       <c r="H3" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="I3" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="Q3" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="T3" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="U3" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="W3" t="s">
-        <v>305</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>48.419957</v>
-      </c>
-      <c r="AG3" t="n">
+        <v>312</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>328</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>329</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE3">
+        <v>48.419956999999997</v>
+      </c>
+      <c r="AG3">
         <v>-123.3688604</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>